<commit_message>
add example website in doc
</commit_message>
<xml_diff>
--- a/docs/techblog_css.xlsx
+++ b/docs/techblog_css.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Example" sheetId="2" r:id="rId2"/>
+    <sheet name="Website" sheetId="3" r:id="rId2"/>
+    <sheet name="Example" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="108">
   <si>
     <t>background-color</t>
   </si>
@@ -188,6 +189,162 @@
   </si>
   <si>
     <t>Black</t>
+  </si>
+  <si>
+    <t>UI Design</t>
+  </si>
+  <si>
+    <t>主页</t>
+  </si>
+  <si>
+    <t>主页大图片形式</t>
+  </si>
+  <si>
+    <t>epam_carbon</t>
+  </si>
+  <si>
+    <t>https://carbon.lab.epam.com/index</t>
+  </si>
+  <si>
+    <t>epam_elements</t>
+  </si>
+  <si>
+    <t>https://elements.epam.com/</t>
+  </si>
+  <si>
+    <t>可作为主页</t>
+  </si>
+  <si>
+    <t>提供visual guidelines</t>
+  </si>
+  <si>
+    <t>http://blackrockdigital.github.io/startbootstrap-landing-page/</t>
+  </si>
+  <si>
+    <t>http://blackrockdigital.github.io/startbootstrap-creative/</t>
+  </si>
+  <si>
+    <t>采用多个元素替代大图片形式</t>
+  </si>
+  <si>
+    <t>epam_sharepoint</t>
+  </si>
+  <si>
+    <t>https://sharepoint.epam.com/Pages/default.aspx</t>
+  </si>
+  <si>
+    <t>不同于主页一个大图片的设计，用多个标签替代大图片，效果也不错，布局也可以借鉴</t>
+  </si>
+  <si>
+    <t>登陆页面</t>
+  </si>
+  <si>
+    <t>其中登陆部分也可用</t>
+  </si>
+  <si>
+    <t>发帖</t>
+  </si>
+  <si>
+    <t>经典左右布局</t>
+  </si>
+  <si>
+    <t>epam_gitlab</t>
+  </si>
+  <si>
+    <t>https://git.epam.com/</t>
+  </si>
+  <si>
+    <t>经典的左右布局，可以作为发帖的参考</t>
+  </si>
+  <si>
+    <t>epam_support</t>
+  </si>
+  <si>
+    <t>https://support.epam.com/esp/ess.do</t>
+  </si>
+  <si>
+    <t>Subtopic 2</t>
+  </si>
+  <si>
+    <t>帖子展示</t>
+  </si>
+  <si>
+    <t>帖子按类型展示</t>
+  </si>
+  <si>
+    <t>采用标签格式</t>
+  </si>
+  <si>
+    <t>epam_events</t>
+  </si>
+  <si>
+    <t>https://events.epam.com/</t>
+  </si>
+  <si>
+    <t>类似于education，可以作为展示topic的页面模板</t>
+  </si>
+  <si>
+    <t>epam_heros</t>
+  </si>
+  <si>
+    <t>https://heroes.epam.com/</t>
+  </si>
+  <si>
+    <t>类似于黏贴板的形式，我们的网站也可以有类似的排行版及奖杯</t>
+  </si>
+  <si>
+    <t>个人主页</t>
+  </si>
+  <si>
+    <t>UPSA</t>
+  </si>
+  <si>
+    <t>工具</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>适合用于发帖记录</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>个人标签</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
+    <t>提供总体页面参考</t>
+  </si>
+  <si>
+    <t>https://www.epam.com/</t>
+  </si>
+  <si>
+    <t>B2bits</t>
+  </si>
+  <si>
+    <t>http://www.b2bits.com/</t>
+  </si>
+  <si>
+    <t>提供鼠标放置上面的图片切换效果</t>
+  </si>
+  <si>
+    <t>可用于论坛主题间的切换</t>
+  </si>
+  <si>
+    <t>signature</t>
+  </si>
+  <si>
+    <t>https://signature.epam.com/</t>
+  </si>
+  <si>
+    <t>不是做ui的，记得download自己的签名</t>
   </si>
 </sst>
 </file>
@@ -344,22 +501,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -800,15 +957,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F22" sqref="F22:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
     <col min="3" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
@@ -816,10 +973,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
@@ -837,73 +994,73 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -912,217 +1069,217 @@
         <v>11</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G20" t="s">
@@ -1130,18 +1287,18 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="9" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G21" t="s">
@@ -1149,76 +1306,88 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="E3:E5"/>
@@ -1235,18 +1404,6 @@
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="E14:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="F7:F12"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C3:C5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
@@ -1257,6 +1414,591 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F114"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:XFD115"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>